<commit_message>
Add products by excel working
</commit_message>
<xml_diff>
--- a/Sample files for testing/Sample.xlsx
+++ b/Sample files for testing/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a01c64a3e96f30f/Documents/Python Projects/Supermarket Management System using Flask and MySQL/Supermarket-Management-System/Sample files for testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC104863A91F52185BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6BB3AC1-754D-4E93-AEDF-2FDAC0CFCAE9}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104863A91F52185BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5644C54-205F-41BC-BF7D-14B731D50430}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4512" yWindow="2856" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Choco</t>
+    <t>Chocolate</t>
   </si>
   <si>
-    <t>Chips</t>
-  </si>
-  <si>
-    <t>31/12/2023</t>
+    <t>Crisp Chips</t>
   </si>
 </sst>
 </file>
@@ -90,6 +87,14 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -359,7 +364,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -372,10 +377,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1324</v>
+        <v>13243</v>
       </c>
       <c r="C1">
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="D1">
         <v>23</v>
@@ -392,19 +397,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>234</v>
+        <v>2346</v>
       </c>
       <c r="C2">
         <v>20</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>18.5</v>
       </c>
       <c r="E2">
         <v>300</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
+      <c r="F2" s="1">
+        <v>45291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything except bill functionality implemented
</commit_message>
<xml_diff>
--- a/Sample files for testing/Sample.xlsx
+++ b/Sample files for testing/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a01c64a3e96f30f/Documents/Python Projects/Supermarket Management System using Flask and MySQL/Supermarket-Management-System/Sample files for testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104863A91F52185BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5644C54-205F-41BC-BF7D-14B731D50430}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC104863A91F52185BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAA13D7E-4A87-4795-BA82-5EE48A1E5FF8}"/>
   <bookViews>
     <workbookView xWindow="4512" yWindow="2856" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Chocolate</t>
+    <t>Chocolate chips</t>
   </si>
   <si>
-    <t>Crisp Chips</t>
+    <t>Crispy bisc</t>
   </si>
 </sst>
 </file>
@@ -95,6 +95,10 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -364,7 +368,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,7 +381,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>13243</v>
+        <v>1300</v>
       </c>
       <c r="C1">
         <v>30.5</v>
@@ -397,7 +401,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2346</v>
+        <v>233124</v>
       </c>
       <c r="C2">
         <v>20</v>

</xml_diff>